<commit_message>
Updated some pin names.
</commit_message>
<xml_diff>
--- a/Firmware.PIC32/firmware/src/Pinout list.xlsx
+++ b/Firmware.PIC32/firmware/src/Pinout list.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14910" windowHeight="10275"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14910" windowHeight="10275"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" calcMode="manual"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -371,9 +370,6 @@
     <t>ZEROR (not used)</t>
   </si>
   <si>
-    <t>PIC32_READY</t>
-  </si>
-  <si>
     <t>CE</t>
   </si>
   <si>
@@ -414,6 +410,9 @@
   </si>
   <si>
     <t>Notifications</t>
+  </si>
+  <si>
+    <t>CMD_NOT_EXEC</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1054,7 @@
   <dimension ref="A1:X65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P31" workbookViewId="0">
-      <selection activeCell="V57" sqref="V57"/>
+      <selection activeCell="AA42" sqref="AA42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,7 +1765,7 @@
         <v>65</v>
       </c>
       <c r="U26" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V26" t="s">
         <v>73</v>
@@ -1810,7 +1809,7 @@
         <v>71</v>
       </c>
       <c r="U30" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V30" t="s">
         <v>73</v>
@@ -1821,7 +1820,7 @@
         <v>63</v>
       </c>
       <c r="U31" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="20:22" x14ac:dyDescent="0.25">
@@ -1888,7 +1887,7 @@
     </row>
     <row r="37" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S37" s="55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T37" s="29" t="s">
         <v>55</v>
@@ -1916,7 +1915,7 @@
     </row>
     <row r="39" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S39" s="55" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="T39" s="29" t="s">
         <v>54</v>
@@ -2009,7 +2008,7 @@
         <v>98</v>
       </c>
       <c r="V50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="19:22" x14ac:dyDescent="0.25">
@@ -2017,35 +2016,35 @@
     </row>
     <row r="54" spans="19:22" x14ac:dyDescent="0.25">
       <c r="S54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T54" s="57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="19:22" x14ac:dyDescent="0.25">
       <c r="S55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T55" s="57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="U55" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="19:22" x14ac:dyDescent="0.25">
       <c r="S56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T56" s="57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="19:22" x14ac:dyDescent="0.25">

</xml_diff>